<commit_message>
import organizations (with structure) and readings from several files
</commit_message>
<xml_diff>
--- a/databases/xlsx/import_all/import 21.05.xlsx
+++ b/databases/xlsx/import_all/import 21.05.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="525">
   <si>
     <t xml:space="preserve">Организация</t>
   </si>
@@ -3202,10 +3202,10 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A198" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="B210" activeCellId="0" sqref="B210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="24.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3215,7 +3215,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="50.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="115.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="138.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="33.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="42.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="47.99"/>
@@ -5517,6 +5517,9 @@
       <c r="H98" s="11" t="n">
         <v>4</v>
       </c>
+      <c r="I98" s="12" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="59"/>
@@ -6447,6 +6450,9 @@
       <c r="H138" s="60" t="n">
         <v>5</v>
       </c>
+      <c r="I138" s="12" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="139" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="74"/>
@@ -7227,6 +7233,9 @@
       <c r="H172" s="75" t="n">
         <v>6</v>
       </c>
+      <c r="I172" s="12" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="173" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="80"/>
@@ -8061,6 +8070,9 @@
       </c>
       <c r="H208" s="81" t="n">
         <v>7</v>
+      </c>
+      <c r="I208" s="12" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8156,7 +8168,7 @@
   </sheetPr>
   <dimension ref="A1:AN56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>

</xml_diff>